<commit_message>
Companies, Contacts & Opp changes - 6th Mar 2024
</commit_message>
<xml_diff>
--- a/TestData/T2238_Contacts_VerifyDuplicateRuleAccountCreatedByAndDupRecordSetOnCreatingDuplicateContactRecords.xlsx
+++ b/TestData/T2238_Contacts_VerifyDuplicateRuleAccountCreatedByAndDupRecordSetOnCreatingDuplicateContactRecords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HL\SalesForce_Project\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03A67BF-67EE-4D5D-A2BD-64D719A23CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0EE827-B7B5-468A-BD3C-0ED88E7703BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>testJames@email.com</t>
-  </si>
-  <si>
     <t>(541) 754-3010</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>ActivityCompany</t>
   </si>
   <si>
-    <t>Drew Koecher</t>
-  </si>
-  <si>
     <t>Folder Name</t>
   </si>
   <si>
@@ -97,13 +91,19 @@
   </si>
   <si>
     <t>Test ExternalContact</t>
+  </si>
+  <si>
+    <t>Ayati Arvind</t>
+  </si>
+  <si>
+    <t>testexternalcontact@email.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +115,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,10 +145,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -150,8 +159,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -432,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +470,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -471,33 +482,33 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -525,24 +536,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -565,7 +576,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -583,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +610,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>